<commit_message>
artigos de metodologia de pesquisa
</commit_message>
<xml_diff>
--- a/Bibliometria1.xlsx
+++ b/Bibliometria1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludmi\Google Drive\Mestrado\Artigo Q-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC68E06-CB4C-4D1B-B388-A446311C66A6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F6381E-9B5C-4FD9-BFB5-391C6049E708}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{892CE944-84D9-4BC9-ABF2-F6D8514C3EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumos" sheetId="2" r:id="rId1"/>
     <sheet name="Lista" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="197">
   <si>
     <t>Autores</t>
   </si>
@@ -623,12 +624,81 @@
   <si>
     <t>O espaço de estados é composto pela  tupla (número de ações de cada ativo,  preço das ações de cada ativo, montante disponível, tendencia de cada ativo estimada pelo modelo markoviano oculto). As ações do agente são representadas por um vetor com a decisao de comprar,vender ou esperar para cada um dos ativos no portfólio. Se o agente decide comprar mais de um ativo, o montande disponível é distribuido igualmente entre eles. Finalmente, as recompensas são devinidas como o valor atual do portfólio.</t>
   </si>
+  <si>
+    <t>Alocação entre ativos de risco  e livre de risco utilizando QL com diferentes funções de otimização: lucro, sharpe ratio. Os parâmetros de alocação são encontrados utilizando método gradiente estocástico</t>
+  </si>
+  <si>
+    <t>O espaço de estados é discrediz</t>
+  </si>
+  <si>
+    <t>Model-based pairs trading in the bitcoin markets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Quantitative Finance</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/full/10.1080/14697688.2016.1231928</t>
+  </si>
+  <si>
+    <t>Hybrid bi-objective portfolio optimization with pre-selection strategy</t>
+  </si>
+  <si>
+    <t>Technology Analysis &amp; Strategic Management</t>
+  </si>
+  <si>
+    <t>Bibliometrics-based evaluation of the Blockchain research trend: 2008 – March 2017</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/full/10.1080/09537325.2018.1434138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+0.960</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0020025517308381</t>
+  </si>
+  <si>
+    <t>Detecting structural changes in large portfolios</t>
+  </si>
+  <si>
+    <t>Empirical Economics</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s00181-017-1392-5</t>
+  </si>
+  <si>
+    <t>0.645</t>
+  </si>
+  <si>
+    <t>Information Sciences</t>
+  </si>
+  <si>
+    <t>Revista</t>
+  </si>
+  <si>
+    <t>Fator de Impacto</t>
+  </si>
+  <si>
+    <t>Qualis</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,6 +716,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -713,10 +791,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -790,8 +869,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1104,42 +1196,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2024F9E3-99B8-401A-992D-7848995BA865}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.08984375" style="23" customWidth="1"/>
     <col min="2" max="2" width="22.1796875" style="23" customWidth="1"/>
-    <col min="3" max="8" width="34.26953125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="34.26953125" style="23" hidden="1" customWidth="1"/>
+    <col min="4" max="8" width="34.26953125" style="23" customWidth="1"/>
     <col min="9" max="16384" width="8.7265625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="27" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1397,66 +1490,84 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" s="17" customFormat="1" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B14" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C14" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D14" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E14" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F14" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G14" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H14" s="24" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="22" t="s">
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B15" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C15" s="24" t="s">
         <v>89</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="J14" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>125</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
+      <c r="J15" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1467,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC7E835-4272-4313-8880-F23D3252DE14}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2349,4 +2460,130 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC67E70-271F-494E-A83F-7EA33BA7CACB}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="5" width="25.81640625" style="1"/>
+    <col min="6" max="16384" width="25.81640625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="26">
+        <v>4832</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{74819888-E466-4EC4-818C-CA3F83986E80}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{22AE01F7-B123-42E5-BB6A-E4031AB26CA4}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{3C14897F-D346-42A1-BD93-62FA590511E2}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{43802558-9D3D-4C16-9FE1-F5142EE0E7EB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>